<commit_message>
continued in prog work
</commit_message>
<xml_diff>
--- a/working/notation_translation_table.xlsx
+++ b/working/notation_translation_table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CBA8C2F2-4C6F-409D-9052-6A4E55D3371E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E5306566-EA33-482D-9C5F-C9322FB7DE10}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
   <si>
     <t>Blei</t>
   </si>
@@ -182,9 +182,6 @@
     <t>κ</t>
   </si>
   <si>
-    <t>ψ</t>
-  </si>
-  <si>
     <t>topicmodels</t>
   </si>
   <si>
@@ -215,9 +212,6 @@
     <t>λ</t>
   </si>
   <si>
-    <t>ι</t>
-  </si>
-  <si>
     <t>γ</t>
   </si>
   <si>
@@ -225,6 +219,27 @@
   </si>
   <si>
     <t>ω</t>
+  </si>
+  <si>
+    <t>η</t>
+  </si>
+  <si>
+    <t>υ</t>
+  </si>
+  <si>
+    <t>organism-level community identity probability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">concentration parameter describing the C-dimensional Dirichlet distribution of organism-level community probabilities within a sample </t>
+  </si>
+  <si>
+    <t>probability describing the S-dimensional categorical distribution of species identity of an organism, given its community identity</t>
+  </si>
+  <si>
+    <t>concentration parameter describing organism-level community identity probability (the community proportion)</t>
+  </si>
+  <si>
+    <t>probability defining the categorical distribution of community identity of individual organisms</t>
   </si>
 </sst>
 </file>
@@ -276,10 +291,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,7 +638,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,18 +652,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
@@ -818,73 +833,88 @@
         <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" t="s">
         <v>56</v>
-      </c>
-      <c r="H14" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C22" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C22" s="2" t="s">
+      <c r="G22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C23" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>63</v>
+      <c r="H23" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aligning notation and tidying code
working through from front to back
LDA functions now all included
need to include tests
</commit_message>
<xml_diff>
--- a/working/notation_translation_table.xlsx
+++ b/working/notation_translation_table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E5306566-EA33-482D-9C5F-C9322FB7DE10}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BD167E95-9B84-4A35-9DC1-AC673D297086}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
   <si>
     <t>Blei</t>
   </si>
@@ -240,6 +240,33 @@
   </si>
   <si>
     <t>probability defining the categorical distribution of community identity of individual organisms</t>
+  </si>
+  <si>
+    <t>ῡ</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">standardized concentration parmater </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>υ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, i.e. organism-level community identity probability</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -635,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -899,6 +926,9 @@
       <c r="C22" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="E22" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="G22" s="1" t="s">
         <v>63</v>
       </c>
@@ -915,6 +945,17 @@
       </c>
       <c r="H23" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H24" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>